<commit_message>
SSE and log-likelihood calculations added
</commit_message>
<xml_diff>
--- a/Combo/UseListed.xlsx
+++ b/Combo/UseListed.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clairemoore-cantwell/GitHub/GSR_Learning/Combo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moore-cantwell\GSRs\Combo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2144A00-2C23-0348-ADED-FD8BE7797C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1DC299-19DC-45DA-8D8B-5ABB7681FD06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7500" yWindow="460" windowWidth="26920" windowHeight="17540" activeTab="2" xr2:uid="{C71280F5-7DBC-4C24-95AC-02E4F36B038E}"/>
+    <workbookView xWindow="7500" yWindow="465" windowWidth="26925" windowHeight="17535" xr2:uid="{C71280F5-7DBC-4C24-95AC-02E4F36B038E}"/>
   </bookViews>
   <sheets>
     <sheet name="Tagalog" sheetId="1" r:id="rId1"/>
     <sheet name="LessListing" sheetId="2" r:id="rId2"/>
     <sheet name="NoListing" sheetId="3" r:id="rId3"/>
+    <sheet name="manualExample" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Tagalog!$E$4:$J$4</definedName>
@@ -50,22 +51,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="70">
   <si>
     <t>input</t>
   </si>
@@ -251,6 +242,30 @@
   </si>
   <si>
     <t>p_listed:</t>
+  </si>
+  <si>
+    <t>lexeme(s)</t>
+  </si>
+  <si>
+    <t>/mot/+/a/</t>
+  </si>
+  <si>
+    <t>/moda/</t>
+  </si>
+  <si>
+    <t>mota</t>
+  </si>
+  <si>
+    <t>moda</t>
+  </si>
+  <si>
+    <t>*VTV</t>
+  </si>
+  <si>
+    <t>Ident-Place</t>
+  </si>
+  <si>
+    <t>useListed</t>
   </si>
 </sst>
 </file>
@@ -816,34 +831,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8924EE5-736F-4A02-BD38-2BDE280E4D14}">
   <dimension ref="A1:T78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="26720" ySplit="1980" topLeftCell="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="26715" ySplit="1980" topLeftCell="L25" activePane="bottomLeft"/>
       <selection sqref="A1:XFD1048576"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:L21"/>
+      <selection pane="bottomLeft" activeCell="S26" sqref="S26"/>
       <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.625" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="26" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="26" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="26" customWidth="1"/>
     <col min="7" max="7" width="9" style="26"/>
-    <col min="8" max="8" width="11.1640625" style="26" customWidth="1"/>
+    <col min="8" max="8" width="11.125" style="26" customWidth="1"/>
     <col min="9" max="9" width="9" style="26"/>
-    <col min="10" max="11" width="9.1640625" style="26" customWidth="1"/>
+    <col min="10" max="11" width="9.125" style="26" customWidth="1"/>
     <col min="12" max="13" width="9" style="26"/>
-    <col min="14" max="14" width="8.1640625" customWidth="1"/>
-    <col min="15" max="15" width="3.33203125" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.125" customWidth="1"/>
+    <col min="15" max="15" width="3.375" customWidth="1"/>
+    <col min="17" max="17" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E1" s="26" t="s">
         <v>34</v>
       </c>
@@ -883,7 +898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -918,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E3" s="26" t="s">
         <v>37</v>
       </c>
@@ -955,7 +970,7 @@
         <v>1.4323793052458513</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -991,7 +1006,7 @@
         <v>5.3523439823050447</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1035,7 +1050,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1079,7 +1094,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -1121,7 +1136,7 @@
       </c>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1163,7 +1178,7 @@
       </c>
       <c r="N8" s="11"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1205,7 +1220,7 @@
       </c>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1247,7 +1262,7 @@
       </c>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1289,7 +1304,7 @@
       </c>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
@@ -1331,7 +1346,7 @@
       </c>
       <c r="N12" s="11"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
@@ -1373,7 +1388,7 @@
       </c>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -1415,7 +1430,7 @@
       </c>
       <c r="N14" s="11"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -1457,7 +1472,7 @@
       </c>
       <c r="N15" s="11"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
@@ -1499,7 +1514,7 @@
       </c>
       <c r="N16" s="11"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -1541,7 +1556,7 @@
       </c>
       <c r="N17" s="11"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -1583,7 +1598,7 @@
       </c>
       <c r="N18" s="11"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -1625,7 +1640,7 @@
       </c>
       <c r="N19" s="11"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>25</v>
       </c>
@@ -1667,7 +1682,7 @@
       </c>
       <c r="N20" s="11"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>25</v>
       </c>
@@ -1709,7 +1724,7 @@
       </c>
       <c r="N21" s="11"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>44</v>
       </c>
@@ -1728,7 +1743,7 @@
         <v>-0.35373305880646</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>38</v>
       </c>
@@ -1789,7 +1804,7 @@
         <v>-1.1765483337050827E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>38</v>
       </c>
@@ -1857,7 +1872,7 @@
         <v>0.29701234288978684</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>38</v>
       </c>
@@ -1925,7 +1940,7 @@
         <v>5.5195613070472316</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>39</v>
       </c>
@@ -1986,7 +2001,7 @@
         <v>-4.6675837959906108</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
@@ -2047,7 +2062,7 @@
         <v>-9.5065697761235624E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>39</v>
       </c>
@@ -2108,7 +2123,7 @@
         <v>-9.6170616829970594</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>40</v>
       </c>
@@ -2169,7 +2184,7 @@
         <v>-1.1765483337050827E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>40</v>
       </c>
@@ -2230,7 +2245,7 @@
         <v>-5.3618266363549196</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>40</v>
       </c>
@@ -2291,7 +2306,7 @@
         <v>-4.9612433703434995</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>41</v>
       </c>
@@ -2352,7 +2367,7 @@
         <v>-4.6675837959906108</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>41</v>
       </c>
@@ -2413,7 +2428,7 @@
         <v>-9.5065697761235624E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>41</v>
       </c>
@@ -2474,7 +2489,7 @@
         <v>-9.6170616829970594</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>42</v>
       </c>
@@ -2535,7 +2550,7 @@
         <v>-4.7366251033306994E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>42</v>
       </c>
@@ -2596,7 +2611,7 @@
         <v>-5.3547977781211999</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>43</v>
       </c>
@@ -2657,7 +2672,7 @@
         <v>-4.6675172108014804</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>43</v>
       </c>
@@ -2718,12 +2733,12 @@
         <v>-9.4399845869936726E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>38</v>
       </c>
@@ -2776,7 +2791,7 @@
         <v>0.98364390425388692</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>38</v>
       </c>
@@ -2836,7 +2851,7 @@
         <v>0.99527431939280187</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>38</v>
       </c>
@@ -2889,7 +2904,7 @@
         <v>6.9711908136891676E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>39</v>
       </c>
@@ -2942,7 +2957,7 @@
         <v>4.7028328710416855E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>39</v>
       </c>
@@ -2995,7 +3010,7 @@
         <v>0.99051619732417462</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>39</v>
       </c>
@@ -3048,7 +3063,7 @@
         <v>3.3329485566007567E-5</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>40</v>
       </c>
@@ -3101,7 +3116,7 @@
         <v>0.98364390425388692</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>40</v>
       </c>
@@ -3154,7 +3169,7 @@
         <v>4.6702041812356132E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>40</v>
       </c>
@@ -3207,7 +3222,7 @@
         <v>6.9711908136891676E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>41</v>
       </c>
@@ -3260,7 +3275,7 @@
         <v>4.7028328710416855E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>41</v>
       </c>
@@ -3313,7 +3328,7 @@
         <v>0.99051619732417462</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>41</v>
       </c>
@@ -3366,7 +3381,7 @@
         <v>3.3329485566007567E-5</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>42</v>
       </c>
@@ -3419,7 +3434,7 @@
         <v>0.99058215322832843</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>42</v>
       </c>
@@ -3472,7 +3487,7 @@
         <v>4.7031460204832913E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="8" t="s">
         <v>43</v>
       </c>
@@ -3525,7 +3540,7 @@
         <v>4.7031460204832913E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="8" t="s">
         <v>43</v>
       </c>
@@ -3578,12 +3593,12 @@
         <v>0.99058215322832843</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>45</v>
       </c>
@@ -3636,7 +3651,7 @@
         <v>0.98830345931592578</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>45</v>
       </c>
@@ -3689,7 +3704,7 @@
         <v>4.692327099335673E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>45</v>
       </c>
@@ -3742,7 +3757,7 @@
         <v>7.0042135847386182E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>46</v>
       </c>
@@ -3795,7 +3810,7 @@
         <v>0.98830345931592578</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>46</v>
       </c>
@@ -3848,7 +3863,7 @@
         <v>4.692327099335673E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>46</v>
       </c>
@@ -3901,7 +3916,7 @@
         <v>7.0042135847386182E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
         <v>47</v>
       </c>
@@ -3954,7 +3969,7 @@
         <v>0.98830345931592578</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>47</v>
       </c>
@@ -4007,7 +4022,7 @@
         <v>4.692327099335673E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
         <v>47</v>
       </c>
@@ -4060,7 +4075,7 @@
         <v>7.0042135847386182E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="6" t="s">
         <v>48</v>
       </c>
@@ -4113,7 +4128,7 @@
         <v>0.98830345931592578</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="6" t="s">
         <v>48</v>
       </c>
@@ -4166,7 +4181,7 @@
         <v>4.692327099335673E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="6" t="s">
         <v>48</v>
       </c>
@@ -4219,7 +4234,7 @@
         <v>7.0042135847386182E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>49</v>
       </c>
@@ -4272,7 +4287,7 @@
         <v>0.99527457501478933</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="7" t="s">
         <v>49</v>
       </c>
@@ -4325,7 +4340,7 @@
         <v>4.7254249852107487E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="8" t="s">
         <v>50</v>
       </c>
@@ -4378,7 +4393,7 @@
         <v>0.99527457501478933</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="8" t="s">
         <v>50</v>
       </c>
@@ -4445,26 +4460,26 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.625" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="26" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="26" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="26"/>
-    <col min="8" max="8" width="11.1640625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="26"/>
-    <col min="10" max="11" width="9.1640625" style="26" customWidth="1"/>
-    <col min="12" max="13" width="8.83203125" style="26"/>
-    <col min="14" max="14" width="8.1640625" customWidth="1"/>
-    <col min="15" max="15" width="3.33203125" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="26"/>
+    <col min="8" max="8" width="11.125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="8.875" style="26"/>
+    <col min="10" max="11" width="9.125" style="26" customWidth="1"/>
+    <col min="12" max="13" width="8.875" style="26"/>
+    <col min="14" max="14" width="8.125" customWidth="1"/>
+    <col min="15" max="15" width="3.375" customWidth="1"/>
+    <col min="17" max="17" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E1" s="26" t="s">
         <v>34</v>
       </c>
@@ -4504,7 +4519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -4539,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E3" s="26" t="s">
         <v>37</v>
       </c>
@@ -4576,7 +4591,7 @@
         <v>1.4323793052458513</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -4612,7 +4627,7 @@
         <v>5.3523439823050447</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -4656,7 +4671,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -4700,7 +4715,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -4742,7 +4757,7 @@
       </c>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -4784,7 +4799,7 @@
       </c>
       <c r="N8" s="11"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -4826,7 +4841,7 @@
       </c>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -4868,7 +4883,7 @@
       </c>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -4910,7 +4925,7 @@
       </c>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
@@ -4952,7 +4967,7 @@
       </c>
       <c r="N12" s="11"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
@@ -4994,7 +5009,7 @@
       </c>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -5036,7 +5051,7 @@
       </c>
       <c r="N14" s="11"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -5078,7 +5093,7 @@
       </c>
       <c r="N15" s="11"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
@@ -5120,7 +5135,7 @@
       </c>
       <c r="N16" s="11"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -5162,7 +5177,7 @@
       </c>
       <c r="N17" s="11"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -5204,7 +5219,7 @@
       </c>
       <c r="N18" s="11"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -5246,7 +5261,7 @@
       </c>
       <c r="N19" s="11"/>
     </row>
-    <row r="20" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>25</v>
       </c>
@@ -5288,7 +5303,7 @@
       </c>
       <c r="N20" s="11"/>
     </row>
-    <row r="21" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>25</v>
       </c>
@@ -5330,7 +5345,7 @@
       </c>
       <c r="N21" s="11"/>
     </row>
-    <row r="23" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -5342,7 +5357,7 @@
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
     </row>
-    <row r="24" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D24" s="60"/>
       <c r="E24" s="60"/>
       <c r="F24" s="60"/>
@@ -5354,7 +5369,7 @@
       <c r="L24" s="60"/>
       <c r="M24" s="60"/>
     </row>
-    <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D25" s="60"/>
       <c r="E25" s="60"/>
       <c r="F25" s="60"/>
@@ -5366,7 +5381,7 @@
       <c r="L25" s="60"/>
       <c r="M25" s="60"/>
     </row>
-    <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D26" s="60"/>
       <c r="E26" s="60"/>
       <c r="F26" s="60"/>
@@ -5378,7 +5393,7 @@
       <c r="L26" s="60"/>
       <c r="M26" s="60"/>
     </row>
-    <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D27" s="60"/>
       <c r="E27" s="60"/>
       <c r="F27" s="60"/>
@@ -5392,7 +5407,7 @@
       <c r="P27" s="61"/>
       <c r="Q27" s="62"/>
     </row>
-    <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D28" s="60"/>
       <c r="E28" s="60"/>
       <c r="F28" s="60"/>
@@ -5405,7 +5420,7 @@
       <c r="M28" s="60"/>
       <c r="Q28" s="63"/>
     </row>
-    <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D29" s="60"/>
       <c r="E29" s="60"/>
       <c r="F29" s="60"/>
@@ -5418,7 +5433,7 @@
       <c r="M29" s="60"/>
       <c r="Q29" s="63"/>
     </row>
-    <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D30" s="60"/>
       <c r="E30" s="60"/>
       <c r="F30" s="60"/>
@@ -5431,7 +5446,7 @@
       <c r="M30" s="60"/>
       <c r="Q30" s="63"/>
     </row>
-    <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D31" s="60"/>
       <c r="E31" s="60"/>
       <c r="F31" s="60"/>
@@ -5445,7 +5460,7 @@
       <c r="P31" s="61"/>
       <c r="Q31" s="62"/>
     </row>
-    <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D32" s="60"/>
       <c r="E32" s="60"/>
       <c r="F32" s="60"/>
@@ -5458,7 +5473,7 @@
       <c r="M32" s="60"/>
       <c r="Q32" s="63"/>
     </row>
-    <row r="33" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D33" s="60"/>
       <c r="E33" s="60"/>
       <c r="F33" s="60"/>
@@ -5472,7 +5487,7 @@
       <c r="P33" s="61"/>
       <c r="Q33" s="62"/>
     </row>
-    <row r="34" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D34" s="60"/>
       <c r="E34" s="60"/>
       <c r="F34" s="60"/>
@@ -5485,7 +5500,7 @@
       <c r="M34" s="60"/>
       <c r="Q34" s="63"/>
     </row>
-    <row r="35" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D35" s="60"/>
       <c r="E35" s="60"/>
       <c r="F35" s="60"/>
@@ -5498,7 +5513,7 @@
       <c r="M35" s="60"/>
       <c r="Q35" s="63"/>
     </row>
-    <row r="36" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D36" s="60"/>
       <c r="E36" s="60"/>
       <c r="F36" s="60"/>
@@ -5511,7 +5526,7 @@
       <c r="M36" s="60"/>
       <c r="Q36" s="63"/>
     </row>
-    <row r="37" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D37" s="60"/>
       <c r="E37" s="60"/>
       <c r="F37" s="60"/>
@@ -5525,7 +5540,7 @@
       <c r="P37" s="61"/>
       <c r="Q37" s="62"/>
     </row>
-    <row r="38" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D38" s="60"/>
       <c r="E38" s="60"/>
       <c r="F38" s="60"/>
@@ -5538,7 +5553,7 @@
       <c r="M38" s="60"/>
       <c r="Q38" s="63"/>
     </row>
-    <row r="39" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D39" s="60"/>
       <c r="E39" s="60"/>
       <c r="F39" s="60"/>
@@ -5552,7 +5567,7 @@
       <c r="P39" s="61"/>
       <c r="Q39" s="62"/>
     </row>
-    <row r="40" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D40" s="60"/>
       <c r="E40" s="60"/>
       <c r="F40" s="60"/>
@@ -5565,7 +5580,7 @@
       <c r="M40" s="60"/>
       <c r="Q40" s="63"/>
     </row>
-    <row r="41" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D41" s="60"/>
       <c r="E41" s="60"/>
       <c r="F41" s="60"/>
@@ -5578,7 +5593,7 @@
       <c r="M41" s="60"/>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D42" s="60"/>
       <c r="E42" s="60"/>
       <c r="F42" s="60"/>
@@ -5592,7 +5607,7 @@
       <c r="P42" s="61"/>
       <c r="Q42" s="62"/>
     </row>
-    <row r="43" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D43" s="60"/>
       <c r="E43" s="60"/>
       <c r="F43" s="60"/>
@@ -5604,7 +5619,7 @@
       <c r="L43" s="60"/>
       <c r="M43" s="60"/>
     </row>
-    <row r="44" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D44" s="60"/>
       <c r="E44" s="60"/>
       <c r="F44" s="60"/>
@@ -5617,7 +5632,7 @@
       <c r="M44" s="60"/>
       <c r="P44" s="61"/>
     </row>
-    <row r="45" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D45" s="60"/>
       <c r="E45" s="60"/>
       <c r="F45" s="60"/>
@@ -5629,7 +5644,7 @@
       <c r="L45" s="60"/>
       <c r="M45" s="60"/>
     </row>
-    <row r="46" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D46" s="60"/>
       <c r="E46" s="60"/>
       <c r="F46" s="60"/>
@@ -5641,7 +5656,7 @@
       <c r="L46" s="60"/>
       <c r="M46" s="60"/>
     </row>
-    <row r="47" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D47" s="60"/>
       <c r="E47" s="60"/>
       <c r="F47" s="60"/>
@@ -5653,7 +5668,7 @@
       <c r="L47" s="60"/>
       <c r="M47" s="60"/>
     </row>
-    <row r="48" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D48" s="60"/>
       <c r="E48" s="60"/>
       <c r="F48" s="60"/>
@@ -5666,7 +5681,7 @@
       <c r="M48" s="60"/>
       <c r="P48" s="61"/>
     </row>
-    <row r="49" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D49" s="60"/>
       <c r="E49" s="60"/>
       <c r="F49" s="60"/>
@@ -5678,7 +5693,7 @@
       <c r="L49" s="60"/>
       <c r="M49" s="60"/>
     </row>
-    <row r="50" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D50" s="60"/>
       <c r="E50" s="60"/>
       <c r="F50" s="60"/>
@@ -5691,7 +5706,7 @@
       <c r="M50" s="60"/>
       <c r="P50" s="61"/>
     </row>
-    <row r="51" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D51" s="60"/>
       <c r="E51" s="60"/>
       <c r="F51" s="60"/>
@@ -5703,7 +5718,7 @@
       <c r="L51" s="60"/>
       <c r="M51" s="60"/>
     </row>
-    <row r="52" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D52" s="60"/>
       <c r="E52" s="60"/>
       <c r="F52" s="60"/>
@@ -5715,7 +5730,7 @@
       <c r="L52" s="60"/>
       <c r="M52" s="60"/>
     </row>
-    <row r="53" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D53" s="60"/>
       <c r="E53" s="60"/>
       <c r="F53" s="60"/>
@@ -5727,7 +5742,7 @@
       <c r="L53" s="60"/>
       <c r="M53" s="60"/>
     </row>
-    <row r="54" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D54" s="60"/>
       <c r="E54" s="60"/>
       <c r="F54" s="60"/>
@@ -5740,7 +5755,7 @@
       <c r="M54" s="60"/>
       <c r="P54" s="61"/>
     </row>
-    <row r="55" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D55" s="60"/>
       <c r="E55" s="60"/>
       <c r="F55" s="60"/>
@@ -5752,7 +5767,7 @@
       <c r="L55" s="60"/>
       <c r="M55" s="60"/>
     </row>
-    <row r="56" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D56" s="60"/>
       <c r="E56" s="60"/>
       <c r="F56" s="60"/>
@@ -5765,7 +5780,7 @@
       <c r="M56" s="60"/>
       <c r="P56" s="61"/>
     </row>
-    <row r="57" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D57" s="60"/>
       <c r="E57" s="60"/>
       <c r="F57" s="60"/>
@@ -5777,7 +5792,7 @@
       <c r="L57" s="60"/>
       <c r="M57" s="60"/>
     </row>
-    <row r="58" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D58" s="60"/>
       <c r="E58" s="60"/>
       <c r="F58" s="60"/>
@@ -5789,7 +5804,7 @@
       <c r="L58" s="60"/>
       <c r="M58" s="60"/>
     </row>
-    <row r="59" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D59" s="60"/>
       <c r="E59" s="60"/>
       <c r="F59" s="60"/>
@@ -5802,7 +5817,7 @@
       <c r="M59" s="60"/>
       <c r="P59" s="61"/>
     </row>
-    <row r="60" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D60" s="60"/>
       <c r="E60" s="60"/>
       <c r="F60" s="60"/>
@@ -5814,7 +5829,7 @@
       <c r="L60" s="60"/>
       <c r="M60" s="60"/>
     </row>
-    <row r="61" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D61" s="60"/>
       <c r="E61" s="60"/>
       <c r="F61" s="60"/>
@@ -5826,7 +5841,7 @@
       <c r="L61" s="60"/>
       <c r="M61" s="60"/>
     </row>
-    <row r="62" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="64"/>
       <c r="D62" s="60"/>
       <c r="E62" s="60"/>
@@ -5839,7 +5854,7 @@
       <c r="L62" s="60"/>
       <c r="M62" s="60"/>
     </row>
-    <row r="63" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D63" s="60"/>
       <c r="E63" s="60"/>
       <c r="F63" s="60"/>
@@ -5852,7 +5867,7 @@
       <c r="M63" s="60"/>
       <c r="P63" s="61"/>
     </row>
-    <row r="64" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D64" s="60"/>
       <c r="E64" s="60"/>
       <c r="F64" s="60"/>
@@ -5864,7 +5879,7 @@
       <c r="L64" s="60"/>
       <c r="M64" s="60"/>
     </row>
-    <row r="65" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D65" s="60"/>
       <c r="E65" s="60"/>
       <c r="F65" s="60"/>
@@ -5876,7 +5891,7 @@
       <c r="L65" s="60"/>
       <c r="M65" s="60"/>
     </row>
-    <row r="66" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D66" s="60"/>
       <c r="E66" s="60"/>
       <c r="F66" s="60"/>
@@ -5888,7 +5903,7 @@
       <c r="L66" s="60"/>
       <c r="M66" s="60"/>
     </row>
-    <row r="67" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D67" s="60"/>
       <c r="E67" s="60"/>
       <c r="F67" s="60"/>
@@ -5901,7 +5916,7 @@
       <c r="M67" s="60"/>
       <c r="P67" s="61"/>
     </row>
-    <row r="68" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D68" s="60"/>
       <c r="E68" s="60"/>
       <c r="F68" s="60"/>
@@ -5913,7 +5928,7 @@
       <c r="L68" s="60"/>
       <c r="M68" s="60"/>
     </row>
-    <row r="69" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D69" s="60"/>
       <c r="E69" s="60"/>
       <c r="F69" s="60"/>
@@ -5926,7 +5941,7 @@
       <c r="M69" s="60"/>
       <c r="P69" s="61"/>
     </row>
-    <row r="70" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D70" s="60"/>
       <c r="E70" s="60"/>
       <c r="F70" s="60"/>
@@ -5938,7 +5953,7 @@
       <c r="L70" s="60"/>
       <c r="M70" s="60"/>
     </row>
-    <row r="71" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D71" s="60"/>
       <c r="E71" s="60"/>
       <c r="F71" s="60"/>
@@ -5950,7 +5965,7 @@
       <c r="L71" s="60"/>
       <c r="M71" s="60"/>
     </row>
-    <row r="72" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D72" s="60"/>
       <c r="E72" s="60"/>
       <c r="F72" s="60"/>
@@ -5962,7 +5977,7 @@
       <c r="L72" s="60"/>
       <c r="M72" s="60"/>
     </row>
-    <row r="73" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D73" s="60"/>
       <c r="E73" s="60"/>
       <c r="F73" s="60"/>
@@ -5975,7 +5990,7 @@
       <c r="M73" s="60"/>
       <c r="P73" s="61"/>
     </row>
-    <row r="74" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D74" s="60"/>
       <c r="E74" s="60"/>
       <c r="F74" s="60"/>
@@ -5987,7 +6002,7 @@
       <c r="L74" s="60"/>
       <c r="M74" s="60"/>
     </row>
-    <row r="75" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D75" s="60"/>
       <c r="E75" s="60"/>
       <c r="F75" s="60"/>
@@ -6000,7 +6015,7 @@
       <c r="M75" s="60"/>
       <c r="P75" s="61"/>
     </row>
-    <row r="76" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D76" s="60"/>
       <c r="E76" s="60"/>
       <c r="F76" s="60"/>
@@ -6012,7 +6027,7 @@
       <c r="L76" s="60"/>
       <c r="M76" s="60"/>
     </row>
-    <row r="77" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D77" s="60"/>
       <c r="E77" s="60"/>
       <c r="F77" s="60"/>
@@ -6024,7 +6039,7 @@
       <c r="L77" s="60"/>
       <c r="M77" s="60"/>
     </row>
-    <row r="78" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D78" s="60"/>
       <c r="E78" s="60"/>
       <c r="F78" s="60"/>
@@ -6037,7 +6052,7 @@
       <c r="M78" s="60"/>
       <c r="P78" s="61"/>
     </row>
-    <row r="79" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D79" s="60"/>
       <c r="E79" s="60"/>
       <c r="F79" s="60"/>
@@ -6049,7 +6064,7 @@
       <c r="L79" s="60"/>
       <c r="M79" s="60"/>
     </row>
-    <row r="80" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D80" s="60"/>
       <c r="E80" s="60"/>
       <c r="F80" s="60"/>
@@ -6061,7 +6076,7 @@
       <c r="L80" s="60"/>
       <c r="M80" s="60"/>
     </row>
-    <row r="81" spans="4:13" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:13" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D81" s="60"/>
       <c r="E81" s="60"/>
       <c r="F81" s="60"/>
@@ -6073,7 +6088,7 @@
       <c r="L81" s="60"/>
       <c r="M81" s="60"/>
     </row>
-    <row r="82" spans="4:13" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:13" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D82" s="60"/>
       <c r="E82" s="60"/>
       <c r="F82" s="60"/>
@@ -6085,7 +6100,7 @@
       <c r="L82" s="60"/>
       <c r="M82" s="60"/>
     </row>
-    <row r="83" spans="4:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D83" s="24"/>
       <c r="E83" s="24"/>
       <c r="F83" s="24"/>
@@ -6097,7 +6112,7 @@
       <c r="L83" s="24"/>
       <c r="M83" s="24"/>
     </row>
-    <row r="84" spans="4:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D84" s="24"/>
       <c r="E84" s="24"/>
       <c r="F84" s="24"/>
@@ -6118,30 +6133,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D32010A3-3C42-2D48-9861-4EE69A54F4EA}">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.625" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="26" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="26" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="26"/>
-    <col min="8" max="8" width="11.1640625" style="26" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="26"/>
-    <col min="10" max="11" width="9.1640625" style="26" customWidth="1"/>
-    <col min="12" max="13" width="8.83203125" style="26"/>
-    <col min="14" max="14" width="8.1640625" customWidth="1"/>
-    <col min="15" max="15" width="3.33203125" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="8.875" style="26"/>
+    <col min="8" max="8" width="11.125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="8.875" style="26"/>
+    <col min="10" max="11" width="9.125" style="26" customWidth="1"/>
+    <col min="12" max="13" width="8.875" style="26"/>
+    <col min="14" max="14" width="8.125" customWidth="1"/>
+    <col min="15" max="15" width="3.375" customWidth="1"/>
+    <col min="17" max="17" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E1" s="26" t="s">
         <v>34</v>
       </c>
@@ -6181,7 +6196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C2" t="s">
         <v>35</v>
       </c>
@@ -6216,7 +6231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E3" s="26" t="s">
         <v>37</v>
       </c>
@@ -6253,7 +6268,7 @@
         <v>1.4323793052458513</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -6289,7 +6304,7 @@
         <v>5.3523439823050447</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -6333,7 +6348,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -6377,7 +6392,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
@@ -6419,7 +6434,7 @@
       </c>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -6461,7 +6476,7 @@
       </c>
       <c r="N8" s="11"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -6503,7 +6518,7 @@
       </c>
       <c r="N9" s="11"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -6545,7 +6560,7 @@
       </c>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -6587,7 +6602,7 @@
       </c>
       <c r="N11" s="11"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>14</v>
       </c>
@@ -6629,7 +6644,7 @@
       </c>
       <c r="N12" s="11"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>14</v>
       </c>
@@ -6671,7 +6686,7 @@
       </c>
       <c r="N13" s="11"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
@@ -6713,7 +6728,7 @@
       </c>
       <c r="N14" s="11"/>
     </row>
-    <row r="15" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -6755,7 +6770,7 @@
       </c>
       <c r="N15" s="11"/>
     </row>
-    <row r="16" spans="1:14" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>21</v>
       </c>
@@ -6797,7 +6812,7 @@
       </c>
       <c r="N16" s="11"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>21</v>
       </c>
@@ -6839,7 +6854,7 @@
       </c>
       <c r="N17" s="11"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
@@ -6881,7 +6896,7 @@
       </c>
       <c r="N18" s="11"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
@@ -6923,7 +6938,7 @@
       </c>
       <c r="N19" s="11"/>
     </row>
-    <row r="20" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>25</v>
       </c>
@@ -6965,7 +6980,7 @@
       </c>
       <c r="N20" s="11"/>
     </row>
-    <row r="21" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="21.75" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>25</v>
       </c>
@@ -7007,7 +7022,7 @@
       </c>
       <c r="N21" s="11"/>
     </row>
-    <row r="23" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -7019,7 +7034,7 @@
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
     </row>
-    <row r="24" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D24" s="60"/>
       <c r="E24" s="60"/>
       <c r="F24" s="60"/>
@@ -7031,7 +7046,7 @@
       <c r="L24" s="60"/>
       <c r="M24" s="60"/>
     </row>
-    <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D25" s="60"/>
       <c r="E25" s="60"/>
       <c r="F25" s="60"/>
@@ -7043,7 +7058,7 @@
       <c r="L25" s="60"/>
       <c r="M25" s="60"/>
     </row>
-    <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D26" s="60"/>
       <c r="E26" s="60"/>
       <c r="F26" s="60"/>
@@ -7055,7 +7070,7 @@
       <c r="L26" s="60"/>
       <c r="M26" s="60"/>
     </row>
-    <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D27" s="60"/>
       <c r="E27" s="60"/>
       <c r="F27" s="60"/>
@@ -7069,7 +7084,7 @@
       <c r="P27" s="61"/>
       <c r="Q27" s="62"/>
     </row>
-    <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D28" s="60"/>
       <c r="E28" s="60"/>
       <c r="F28" s="60"/>
@@ -7082,7 +7097,7 @@
       <c r="M28" s="60"/>
       <c r="Q28" s="63"/>
     </row>
-    <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D29" s="60"/>
       <c r="E29" s="60"/>
       <c r="F29" s="60"/>
@@ -7095,7 +7110,7 @@
       <c r="M29" s="60"/>
       <c r="Q29" s="63"/>
     </row>
-    <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D30" s="60"/>
       <c r="E30" s="60"/>
       <c r="F30" s="60"/>
@@ -7108,7 +7123,7 @@
       <c r="M30" s="60"/>
       <c r="Q30" s="63"/>
     </row>
-    <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D31" s="60"/>
       <c r="E31" s="60"/>
       <c r="F31" s="60"/>
@@ -7122,7 +7137,7 @@
       <c r="P31" s="61"/>
       <c r="Q31" s="62"/>
     </row>
-    <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D32" s="60"/>
       <c r="E32" s="60"/>
       <c r="F32" s="60"/>
@@ -7135,7 +7150,7 @@
       <c r="M32" s="60"/>
       <c r="Q32" s="63"/>
     </row>
-    <row r="33" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D33" s="60"/>
       <c r="E33" s="60"/>
       <c r="F33" s="60"/>
@@ -7149,7 +7164,7 @@
       <c r="P33" s="61"/>
       <c r="Q33" s="62"/>
     </row>
-    <row r="34" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D34" s="60"/>
       <c r="E34" s="60"/>
       <c r="F34" s="60"/>
@@ -7162,7 +7177,7 @@
       <c r="M34" s="60"/>
       <c r="Q34" s="63"/>
     </row>
-    <row r="35" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D35" s="60"/>
       <c r="E35" s="60"/>
       <c r="F35" s="60"/>
@@ -7175,7 +7190,7 @@
       <c r="M35" s="60"/>
       <c r="Q35" s="63"/>
     </row>
-    <row r="36" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D36" s="60"/>
       <c r="E36" s="60"/>
       <c r="F36" s="60"/>
@@ -7188,7 +7203,7 @@
       <c r="M36" s="60"/>
       <c r="Q36" s="63"/>
     </row>
-    <row r="37" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D37" s="60"/>
       <c r="E37" s="60"/>
       <c r="F37" s="60"/>
@@ -7202,7 +7217,7 @@
       <c r="P37" s="61"/>
       <c r="Q37" s="62"/>
     </row>
-    <row r="38" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D38" s="60"/>
       <c r="E38" s="60"/>
       <c r="F38" s="60"/>
@@ -7215,7 +7230,7 @@
       <c r="M38" s="60"/>
       <c r="Q38" s="63"/>
     </row>
-    <row r="39" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D39" s="60"/>
       <c r="E39" s="60"/>
       <c r="F39" s="60"/>
@@ -7229,7 +7244,7 @@
       <c r="P39" s="61"/>
       <c r="Q39" s="62"/>
     </row>
-    <row r="40" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D40" s="60"/>
       <c r="E40" s="60"/>
       <c r="F40" s="60"/>
@@ -7242,7 +7257,7 @@
       <c r="M40" s="60"/>
       <c r="Q40" s="63"/>
     </row>
-    <row r="41" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D41" s="60"/>
       <c r="E41" s="60"/>
       <c r="F41" s="60"/>
@@ -7255,7 +7270,7 @@
       <c r="M41" s="60"/>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D42" s="60"/>
       <c r="E42" s="60"/>
       <c r="F42" s="60"/>
@@ -7269,7 +7284,7 @@
       <c r="P42" s="61"/>
       <c r="Q42" s="62"/>
     </row>
-    <row r="43" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D43" s="60"/>
       <c r="E43" s="60"/>
       <c r="F43" s="60"/>
@@ -7281,7 +7296,7 @@
       <c r="L43" s="60"/>
       <c r="M43" s="60"/>
     </row>
-    <row r="44" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D44" s="60"/>
       <c r="E44" s="60"/>
       <c r="F44" s="60"/>
@@ -7294,7 +7309,7 @@
       <c r="M44" s="60"/>
       <c r="P44" s="61"/>
     </row>
-    <row r="45" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D45" s="60"/>
       <c r="E45" s="60"/>
       <c r="F45" s="60"/>
@@ -7306,7 +7321,7 @@
       <c r="L45" s="60"/>
       <c r="M45" s="60"/>
     </row>
-    <row r="46" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D46" s="60"/>
       <c r="E46" s="60"/>
       <c r="F46" s="60"/>
@@ -7318,7 +7333,7 @@
       <c r="L46" s="60"/>
       <c r="M46" s="60"/>
     </row>
-    <row r="47" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D47" s="60"/>
       <c r="E47" s="60"/>
       <c r="F47" s="60"/>
@@ -7330,7 +7345,7 @@
       <c r="L47" s="60"/>
       <c r="M47" s="60"/>
     </row>
-    <row r="48" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:17" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D48" s="60"/>
       <c r="E48" s="60"/>
       <c r="F48" s="60"/>
@@ -7343,7 +7358,7 @@
       <c r="M48" s="60"/>
       <c r="P48" s="61"/>
     </row>
-    <row r="49" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D49" s="60"/>
       <c r="E49" s="60"/>
       <c r="F49" s="60"/>
@@ -7355,7 +7370,7 @@
       <c r="L49" s="60"/>
       <c r="M49" s="60"/>
     </row>
-    <row r="50" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D50" s="60"/>
       <c r="E50" s="60"/>
       <c r="F50" s="60"/>
@@ -7368,7 +7383,7 @@
       <c r="M50" s="60"/>
       <c r="P50" s="61"/>
     </row>
-    <row r="51" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D51" s="60"/>
       <c r="E51" s="60"/>
       <c r="F51" s="60"/>
@@ -7380,7 +7395,7 @@
       <c r="L51" s="60"/>
       <c r="M51" s="60"/>
     </row>
-    <row r="52" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D52" s="60"/>
       <c r="E52" s="60"/>
       <c r="F52" s="60"/>
@@ -7392,7 +7407,7 @@
       <c r="L52" s="60"/>
       <c r="M52" s="60"/>
     </row>
-    <row r="53" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D53" s="60"/>
       <c r="E53" s="60"/>
       <c r="F53" s="60"/>
@@ -7404,7 +7419,7 @@
       <c r="L53" s="60"/>
       <c r="M53" s="60"/>
     </row>
-    <row r="54" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D54" s="60"/>
       <c r="E54" s="60"/>
       <c r="F54" s="60"/>
@@ -7417,7 +7432,7 @@
       <c r="M54" s="60"/>
       <c r="P54" s="61"/>
     </row>
-    <row r="55" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D55" s="60"/>
       <c r="E55" s="60"/>
       <c r="F55" s="60"/>
@@ -7429,7 +7444,7 @@
       <c r="L55" s="60"/>
       <c r="M55" s="60"/>
     </row>
-    <row r="56" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D56" s="60"/>
       <c r="E56" s="60"/>
       <c r="F56" s="60"/>
@@ -7442,7 +7457,7 @@
       <c r="M56" s="60"/>
       <c r="P56" s="61"/>
     </row>
-    <row r="57" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D57" s="60"/>
       <c r="E57" s="60"/>
       <c r="F57" s="60"/>
@@ -7454,7 +7469,7 @@
       <c r="L57" s="60"/>
       <c r="M57" s="60"/>
     </row>
-    <row r="58" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D58" s="60"/>
       <c r="E58" s="60"/>
       <c r="F58" s="60"/>
@@ -7466,7 +7481,7 @@
       <c r="L58" s="60"/>
       <c r="M58" s="60"/>
     </row>
-    <row r="59" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D59" s="60"/>
       <c r="E59" s="60"/>
       <c r="F59" s="60"/>
@@ -7479,7 +7494,7 @@
       <c r="M59" s="60"/>
       <c r="P59" s="61"/>
     </row>
-    <row r="60" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D60" s="60"/>
       <c r="E60" s="60"/>
       <c r="F60" s="60"/>
@@ -7491,7 +7506,7 @@
       <c r="L60" s="60"/>
       <c r="M60" s="60"/>
     </row>
-    <row r="61" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D61" s="60"/>
       <c r="E61" s="60"/>
       <c r="F61" s="60"/>
@@ -7503,7 +7518,7 @@
       <c r="L61" s="60"/>
       <c r="M61" s="60"/>
     </row>
-    <row r="62" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="64"/>
       <c r="D62" s="60"/>
       <c r="E62" s="60"/>
@@ -7516,7 +7531,7 @@
       <c r="L62" s="60"/>
       <c r="M62" s="60"/>
     </row>
-    <row r="63" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D63" s="60"/>
       <c r="E63" s="60"/>
       <c r="F63" s="60"/>
@@ -7529,7 +7544,7 @@
       <c r="M63" s="60"/>
       <c r="P63" s="61"/>
     </row>
-    <row r="64" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D64" s="60"/>
       <c r="E64" s="60"/>
       <c r="F64" s="60"/>
@@ -7541,7 +7556,7 @@
       <c r="L64" s="60"/>
       <c r="M64" s="60"/>
     </row>
-    <row r="65" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D65" s="60"/>
       <c r="E65" s="60"/>
       <c r="F65" s="60"/>
@@ -7553,7 +7568,7 @@
       <c r="L65" s="60"/>
       <c r="M65" s="60"/>
     </row>
-    <row r="66" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D66" s="60"/>
       <c r="E66" s="60"/>
       <c r="F66" s="60"/>
@@ -7565,7 +7580,7 @@
       <c r="L66" s="60"/>
       <c r="M66" s="60"/>
     </row>
-    <row r="67" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D67" s="60"/>
       <c r="E67" s="60"/>
       <c r="F67" s="60"/>
@@ -7578,7 +7593,7 @@
       <c r="M67" s="60"/>
       <c r="P67" s="61"/>
     </row>
-    <row r="68" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D68" s="60"/>
       <c r="E68" s="60"/>
       <c r="F68" s="60"/>
@@ -7590,7 +7605,7 @@
       <c r="L68" s="60"/>
       <c r="M68" s="60"/>
     </row>
-    <row r="69" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D69" s="60"/>
       <c r="E69" s="60"/>
       <c r="F69" s="60"/>
@@ -7603,7 +7618,7 @@
       <c r="M69" s="60"/>
       <c r="P69" s="61"/>
     </row>
-    <row r="70" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D70" s="60"/>
       <c r="E70" s="60"/>
       <c r="F70" s="60"/>
@@ -7615,7 +7630,7 @@
       <c r="L70" s="60"/>
       <c r="M70" s="60"/>
     </row>
-    <row r="71" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D71" s="60"/>
       <c r="E71" s="60"/>
       <c r="F71" s="60"/>
@@ -7627,7 +7642,7 @@
       <c r="L71" s="60"/>
       <c r="M71" s="60"/>
     </row>
-    <row r="72" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D72" s="60"/>
       <c r="E72" s="60"/>
       <c r="F72" s="60"/>
@@ -7639,7 +7654,7 @@
       <c r="L72" s="60"/>
       <c r="M72" s="60"/>
     </row>
-    <row r="73" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D73" s="60"/>
       <c r="E73" s="60"/>
       <c r="F73" s="60"/>
@@ -7652,7 +7667,7 @@
       <c r="M73" s="60"/>
       <c r="P73" s="61"/>
     </row>
-    <row r="74" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D74" s="60"/>
       <c r="E74" s="60"/>
       <c r="F74" s="60"/>
@@ -7664,7 +7679,7 @@
       <c r="L74" s="60"/>
       <c r="M74" s="60"/>
     </row>
-    <row r="75" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D75" s="60"/>
       <c r="E75" s="60"/>
       <c r="F75" s="60"/>
@@ -7677,7 +7692,7 @@
       <c r="M75" s="60"/>
       <c r="P75" s="61"/>
     </row>
-    <row r="76" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D76" s="60"/>
       <c r="E76" s="60"/>
       <c r="F76" s="60"/>
@@ -7689,7 +7704,7 @@
       <c r="L76" s="60"/>
       <c r="M76" s="60"/>
     </row>
-    <row r="77" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D77" s="60"/>
       <c r="E77" s="60"/>
       <c r="F77" s="60"/>
@@ -7701,7 +7716,7 @@
       <c r="L77" s="60"/>
       <c r="M77" s="60"/>
     </row>
-    <row r="78" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D78" s="60"/>
       <c r="E78" s="60"/>
       <c r="F78" s="60"/>
@@ -7714,7 +7729,7 @@
       <c r="M78" s="60"/>
       <c r="P78" s="61"/>
     </row>
-    <row r="79" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D79" s="60"/>
       <c r="E79" s="60"/>
       <c r="F79" s="60"/>
@@ -7726,7 +7741,7 @@
       <c r="L79" s="60"/>
       <c r="M79" s="60"/>
     </row>
-    <row r="80" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="4:16" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D80" s="60"/>
       <c r="E80" s="60"/>
       <c r="F80" s="60"/>
@@ -7738,7 +7753,7 @@
       <c r="L80" s="60"/>
       <c r="M80" s="60"/>
     </row>
-    <row r="81" spans="4:13" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:13" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D81" s="60"/>
       <c r="E81" s="60"/>
       <c r="F81" s="60"/>
@@ -7750,7 +7765,7 @@
       <c r="L81" s="60"/>
       <c r="M81" s="60"/>
     </row>
-    <row r="82" spans="4:13" s="59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:13" s="59" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D82" s="60"/>
       <c r="E82" s="60"/>
       <c r="F82" s="60"/>
@@ -7762,7 +7777,7 @@
       <c r="L82" s="60"/>
       <c r="M82" s="60"/>
     </row>
-    <row r="83" spans="4:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D83" s="24"/>
       <c r="E83" s="24"/>
       <c r="F83" s="24"/>
@@ -7774,7 +7789,7 @@
       <c r="L83" s="24"/>
       <c r="M83" s="24"/>
     </row>
-    <row r="84" spans="4:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D84" s="24"/>
       <c r="E84" s="24"/>
       <c r="F84" s="24"/>
@@ -7789,4 +7804,327 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B0C6AC-BB49-4482-AEF6-AF2AF55783BE}">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="26">
+        <f>(E4-E2)*SQRT(2)/$C$2^2</f>
+        <v>1.4142135623730951E-2</v>
+      </c>
+      <c r="F1" s="26">
+        <f t="shared" ref="F1:L1" si="0">(F4-F2)*SQRT(2)/$C$2^2</f>
+        <v>2.8284271247461901E-2</v>
+      </c>
+      <c r="G1" s="26">
+        <f t="shared" si="0"/>
+        <v>1.4142135623730951E-2</v>
+      </c>
+      <c r="H1" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I1" s="26">
+        <f t="shared" si="0"/>
+        <v>7.5661290421233096E-2</v>
+      </c>
+      <c r="J1" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K1" s="26">
+        <f t="shared" si="0"/>
+        <v>7.5661290421233096E-2</v>
+      </c>
+      <c r="L1" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="26">
+        <v>10</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="26">
+        <v>0</v>
+      </c>
+      <c r="F2" s="26">
+        <v>0</v>
+      </c>
+      <c r="G2" s="26">
+        <v>0</v>
+      </c>
+      <c r="H2" s="26">
+        <v>0</v>
+      </c>
+      <c r="I2" s="26">
+        <v>0</v>
+      </c>
+      <c r="J2" s="26">
+        <v>0</v>
+      </c>
+      <c r="K2" s="27">
+        <v>0</v>
+      </c>
+      <c r="L2" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="26">
+        <f>(E4-E2)^2/2/$C$2</f>
+        <v>0.05</v>
+      </c>
+      <c r="F3" s="26">
+        <f t="shared" ref="F3:L3" si="1">(F4-F2)^2/2/$C$2</f>
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="26">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="H3" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I3" s="26">
+        <f t="shared" si="1"/>
+        <v>1.4311577170515444</v>
+      </c>
+      <c r="J3" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K3" s="26">
+        <f t="shared" si="1"/>
+        <v>1.4311577170515444</v>
+      </c>
+      <c r="L3" s="26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>5.3500611530178688</v>
+      </c>
+      <c r="J4" s="3">
+        <f>H4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <f>I4</f>
+        <v>5.3500611530178688</v>
+      </c>
+      <c r="L4" s="24">
+        <f>D4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="29">
+        <v>0</v>
+      </c>
+      <c r="D6" s="29">
+        <v>10</v>
+      </c>
+      <c r="E6" s="29">
+        <v>1</v>
+      </c>
+      <c r="F6" s="29">
+        <v>0</v>
+      </c>
+      <c r="G6" s="29">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <f>-SUMPRODUCT(E6:G6,E$4:G$4)</f>
+        <v>-2</v>
+      </c>
+      <c r="I6">
+        <f>EXP(H6)</f>
+        <v>0.1353352832366127</v>
+      </c>
+      <c r="J6">
+        <f>I6/SUM(I$6:I$9)</f>
+        <v>0.10959126317106233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="29">
+        <v>1</v>
+      </c>
+      <c r="D7" s="29">
+        <v>10</v>
+      </c>
+      <c r="E7" s="29">
+        <v>0</v>
+      </c>
+      <c r="F7" s="29">
+        <v>1</v>
+      </c>
+      <c r="G7" s="29">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H9" si="2">-SUMPRODUCT(E7:G7,E$4:G$4)</f>
+        <v>-3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ref="I7:I9" si="3">EXP(H7)</f>
+        <v>4.9787068367863944E-2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7:J9" si="4">I7/SUM(I$6:I$9)</f>
+        <v>4.0316372652642873E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="29">
+        <v>0</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29">
+        <v>1</v>
+      </c>
+      <c r="F8" s="29">
+        <v>1</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>4.9787068367863944E-2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="4"/>
+        <v>4.0316372652642873E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="29">
+        <v>1</v>
+      </c>
+      <c r="D9" s="29">
+        <v>10</v>
+      </c>
+      <c r="E9" s="29">
+        <v>0</v>
+      </c>
+      <c r="F9" s="29">
+        <v>0</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="4"/>
+        <v>0.80977599152365198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>